<commit_message>
Another small update :)
</commit_message>
<xml_diff>
--- a/Files/General/Tables/Equipment/Exotic/Exotic Armors.xlsx
+++ b/Files/General/Tables/Equipment/Exotic/Exotic Armors.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="190">
   <si>
     <t>ARMORS</t>
   </si>
@@ -321,9 +321,6 @@
     <t>Dominion Gilded Buckler</t>
   </si>
   <si>
-    <t>Psijic Mystical Aegis</t>
-  </si>
-  <si>
     <t>Aedric Heavenly Helm</t>
   </si>
   <si>
@@ -423,33 +420,6 @@
     <t>Ancient Yokudan Ansei Buckler</t>
   </si>
   <si>
-    <t>Psijic Mystical Helmet</t>
-  </si>
-  <si>
-    <t>Psijic Mystical Cuirass</t>
-  </si>
-  <si>
-    <t>Psijic Mystical Gauntlets</t>
-  </si>
-  <si>
-    <t>Psijic Mystical Boots</t>
-  </si>
-  <si>
-    <t>Psijic Mystical Mail</t>
-  </si>
-  <si>
-    <t>Psijic Mystical Gloves</t>
-  </si>
-  <si>
-    <t>Psijic Mystical Footwear</t>
-  </si>
-  <si>
-    <t>Psijic Mystical Head</t>
-  </si>
-  <si>
-    <t>Psijic Mystical Buckler</t>
-  </si>
-  <si>
     <t>Ancient Direnni Adamantium Helm</t>
   </si>
   <si>
@@ -649,6 +619,21 @@
   </si>
   <si>
     <t>Ancient Yokudan Ansei Headgear</t>
+  </si>
+  <si>
+    <t>Psijic Warden Helmet</t>
+  </si>
+  <si>
+    <t>Psijic Warden Cuirass</t>
+  </si>
+  <si>
+    <t>Psijic Warden Gauntlets</t>
+  </si>
+  <si>
+    <t>Psijic Warden Boots</t>
+  </si>
+  <si>
+    <t>Psijic Warden Aegis</t>
   </si>
 </sst>
 </file>
@@ -1068,10 +1053,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:L184"/>
+  <dimension ref="B1:L179"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="C78" sqref="B75:C78"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="F91" sqref="F91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1146,7 +1131,7 @@
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C9" t="s">
         <v>30</v>
@@ -1154,7 +1139,7 @@
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C10" t="s">
         <v>31</v>
@@ -1162,7 +1147,7 @@
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C11" t="s">
         <v>32</v>
@@ -1170,7 +1155,7 @@
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C12" t="s">
         <v>33</v>
@@ -1179,7 +1164,7 @@
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C13" t="s">
         <v>34</v>
@@ -1187,7 +1172,7 @@
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>194</v>
+        <v>184</v>
       </c>
       <c r="C14" t="s">
         <v>35</v>
@@ -1195,7 +1180,7 @@
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C15" t="s">
         <v>36</v>
@@ -1203,7 +1188,7 @@
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C16" t="s">
         <v>37</v>
@@ -1211,7 +1196,7 @@
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C17" t="s">
         <v>38</v>
@@ -1219,7 +1204,7 @@
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C18" t="s">
         <v>39</v>
@@ -1515,7 +1500,7 @@
     </row>
     <row r="55" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="C55" t="s">
         <v>30</v>
@@ -1523,7 +1508,7 @@
     </row>
     <row r="56" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="C56" t="s">
         <v>31</v>
@@ -1531,7 +1516,7 @@
     </row>
     <row r="57" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="C57" t="s">
         <v>32</v>
@@ -1539,7 +1524,7 @@
     </row>
     <row r="58" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="C58" t="s">
         <v>33</v>
@@ -1611,7 +1596,7 @@
     </row>
     <row r="67" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C67" t="s">
         <v>30</v>
@@ -1619,7 +1604,7 @@
     </row>
     <row r="68" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C68" t="s">
         <v>31</v>
@@ -1627,7 +1612,7 @@
     </row>
     <row r="69" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C69" t="s">
         <v>32</v>
@@ -1635,7 +1620,7 @@
     </row>
     <row r="70" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C70" t="s">
         <v>33</v>
@@ -1643,7 +1628,7 @@
     </row>
     <row r="71" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C71" t="s">
         <v>35</v>
@@ -1651,7 +1636,7 @@
     </row>
     <row r="72" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C72" t="s">
         <v>36</v>
@@ -1659,7 +1644,7 @@
     </row>
     <row r="73" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C73" t="s">
         <v>37</v>
@@ -1667,7 +1652,7 @@
     </row>
     <row r="74" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C74" t="s">
         <v>38</v>
@@ -1675,7 +1660,7 @@
     </row>
     <row r="75" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="C75" t="s">
         <v>35</v>
@@ -1683,7 +1668,7 @@
     </row>
     <row r="76" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="C76" t="s">
         <v>36</v>
@@ -1691,7 +1676,7 @@
     </row>
     <row r="77" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="C77" t="s">
         <v>37</v>
@@ -1699,7 +1684,7 @@
     </row>
     <row r="78" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="C78" t="s">
         <v>38</v>
@@ -1727,7 +1712,7 @@
     </row>
     <row r="83" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
-        <v>119</v>
+        <v>185</v>
       </c>
       <c r="C83" t="s">
         <v>30</v>
@@ -1735,7 +1720,7 @@
     </row>
     <row r="84" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
-        <v>120</v>
+        <v>186</v>
       </c>
       <c r="C84" t="s">
         <v>31</v>
@@ -1743,7 +1728,7 @@
     </row>
     <row r="85" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
-        <v>121</v>
+        <v>187</v>
       </c>
       <c r="C85" t="s">
         <v>32</v>
@@ -1751,7 +1736,7 @@
     </row>
     <row r="86" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
-        <v>122</v>
+        <v>188</v>
       </c>
       <c r="C86" t="s">
         <v>33</v>
@@ -1759,7 +1744,7 @@
     </row>
     <row r="87" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
-        <v>85</v>
+        <v>189</v>
       </c>
       <c r="C87" t="s">
         <v>34</v>
@@ -1767,264 +1752,264 @@
     </row>
     <row r="88" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
-        <v>126</v>
-      </c>
-      <c r="C88" t="s">
-        <v>35</v>
+        <v>54</v>
       </c>
     </row>
     <row r="89" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
-        <v>123</v>
-      </c>
-      <c r="C89" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
     </row>
     <row r="90" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B90" t="s">
-        <v>124</v>
-      </c>
-      <c r="C90" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
     </row>
     <row r="91" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
-        <v>125</v>
-      </c>
-      <c r="C91" t="s">
-        <v>38</v>
+        <v>54</v>
       </c>
     </row>
     <row r="92" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
-        <v>127</v>
-      </c>
-      <c r="C92" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
     </row>
     <row r="93" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B93" t="s">
-        <v>54</v>
+        <v>55</v>
+      </c>
+      <c r="C93" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="94" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
-        <v>54</v>
+        <v>56</v>
+      </c>
+      <c r="C94" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="95" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B95" t="s">
-        <v>54</v>
+        <v>58</v>
+      </c>
+      <c r="C95" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="96" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B96" t="s">
-        <v>54</v>
+        <v>57</v>
+      </c>
+      <c r="C96" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="97" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B97" t="s">
-        <v>54</v>
+        <v>61</v>
+      </c>
+      <c r="C97" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="98" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B98" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="C98" t="s">
-        <v>69</v>
+        <v>31</v>
       </c>
     </row>
     <row r="99" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B99" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="C99" t="s">
-        <v>70</v>
+        <v>32</v>
       </c>
     </row>
     <row r="100" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B100" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="C100" t="s">
-        <v>71</v>
+        <v>33</v>
       </c>
     </row>
     <row r="101" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B101" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C101" t="s">
-        <v>72</v>
+        <v>34</v>
       </c>
     </row>
     <row r="102" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B102" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="C102" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
     </row>
     <row r="103" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B103" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C103" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
     </row>
     <row r="104" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B104" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="C104" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
     <row r="105" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B105" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C105" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
     </row>
     <row r="106" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B106" t="s">
-        <v>59</v>
+        <v>85</v>
       </c>
       <c r="C106" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="107" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B107" t="s">
-        <v>65</v>
+        <v>86</v>
       </c>
       <c r="C107" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="108" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B108" t="s">
-        <v>62</v>
+        <v>87</v>
       </c>
       <c r="C108" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="109" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B109" t="s">
-        <v>66</v>
+        <v>88</v>
       </c>
       <c r="C109" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="110" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B110" t="s">
-        <v>67</v>
+        <v>89</v>
       </c>
       <c r="C110" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="111" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B111" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="C111" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
     </row>
     <row r="112" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B112" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="C112" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
     </row>
     <row r="113" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B113" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="C113" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
     <row r="114" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B114" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="C114" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
     </row>
     <row r="115" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B115" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="C115" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
     </row>
     <row r="116" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B116" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="C116" t="s">
-        <v>35</v>
+        <v>82</v>
       </c>
     </row>
     <row r="117" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B117" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="C117" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="118" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B118" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="C118" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="119" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B119" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="C119" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="120" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B120" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="C120" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="121" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B121" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="C121" t="s">
-        <v>82</v>
+        <v>34</v>
       </c>
     </row>
     <row r="122" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B122" t="s">
-        <v>97</v>
+        <v>118</v>
       </c>
       <c r="C122" t="s">
         <v>30</v>
@@ -2032,7 +2017,7 @@
     </row>
     <row r="123" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B123" t="s">
-        <v>98</v>
+        <v>119</v>
       </c>
       <c r="C123" t="s">
         <v>31</v>
@@ -2040,7 +2025,7 @@
     </row>
     <row r="124" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B124" t="s">
-        <v>99</v>
+        <v>120</v>
       </c>
       <c r="C124" t="s">
         <v>32</v>
@@ -2048,7 +2033,7 @@
     </row>
     <row r="125" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B125" t="s">
-        <v>100</v>
+        <v>121</v>
       </c>
       <c r="C125" t="s">
         <v>33</v>
@@ -2056,7 +2041,7 @@
     </row>
     <row r="126" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B126" t="s">
-        <v>101</v>
+        <v>122</v>
       </c>
       <c r="C126" t="s">
         <v>34</v>
@@ -2064,319 +2049,279 @@
     </row>
     <row r="127" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B127" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="C127" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
     </row>
     <row r="128" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B128" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="C128" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
     </row>
     <row r="129" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B129" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="C129" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
     <row r="130" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B130" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="C130" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
     </row>
     <row r="131" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B131" t="s">
-        <v>132</v>
-      </c>
-      <c r="C131" t="s">
-        <v>34</v>
+        <v>127</v>
       </c>
     </row>
     <row r="132" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B132" t="s">
-        <v>133</v>
-      </c>
-      <c r="C132" t="s">
-        <v>35</v>
+        <v>128</v>
       </c>
     </row>
     <row r="133" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B133" t="s">
-        <v>134</v>
-      </c>
-      <c r="C133" t="s">
-        <v>36</v>
+        <v>129</v>
       </c>
     </row>
     <row r="134" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B134" t="s">
-        <v>135</v>
-      </c>
-      <c r="C134" t="s">
-        <v>37</v>
+        <v>130</v>
       </c>
     </row>
     <row r="135" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B135" t="s">
-        <v>136</v>
-      </c>
-      <c r="C135" t="s">
-        <v>38</v>
+        <v>131</v>
       </c>
     </row>
     <row r="136" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B136" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
     </row>
     <row r="137" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B137" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
     </row>
     <row r="138" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B138" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
     </row>
     <row r="139" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B139" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
     </row>
     <row r="140" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B140" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
     </row>
     <row r="141" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B141" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
     </row>
     <row r="142" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B142" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
     </row>
     <row r="143" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B143" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
     </row>
     <row r="144" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B144" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
     </row>
     <row r="145" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B145" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
     </row>
     <row r="146" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B146" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="147" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B147" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="148" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B148" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="149" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B149" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="150" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B150" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="151" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B151" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
     </row>
     <row r="152" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B152" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
     </row>
     <row r="153" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B153" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="154" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B154" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
     </row>
     <row r="155" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B155" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="156" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B156" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
     </row>
     <row r="157" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B157" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="158" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B158" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
     </row>
     <row r="159" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B159" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="160" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B160" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
     </row>
     <row r="161" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B161" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="162" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B162" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
     </row>
     <row r="163" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B163" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
     </row>
     <row r="164" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B164" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
     </row>
     <row r="165" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B165" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
     </row>
     <row r="166" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B166" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
     </row>
     <row r="167" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B167" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="168" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B168" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="169" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B169" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="170" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B170" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
     </row>
     <row r="171" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B171" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="172" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B172" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
     </row>
     <row r="173" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B173" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
     </row>
     <row r="174" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B174" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
     </row>
     <row r="175" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B175" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
     </row>
     <row r="176" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B176" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
     </row>
     <row r="177" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B177" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
     </row>
     <row r="178" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B178" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
     </row>
     <row r="179" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B179" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="180" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B180" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="181" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B181" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="182" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B182" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="183" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B183" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="184" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B184" t="s">
-        <v>193</v>
+        <v>183</v>
       </c>
     </row>
   </sheetData>

</xml_diff>